<commit_message>
add detekt report and update checklist
</commit_message>
<xml_diff>
--- a/Documents/BitriseSteps.xlsx
+++ b/Documents/BitriseSteps.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FH Campus Wien\6.Semester\Bachelorarbeit 2\Arbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D97E144E-E29C-4809-8118-4A1A820D5EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77837E94-3C2F-4B98-8F95-1C422058A279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{91CF1E20-E424-4D3E-8CFC-94115AA2DE71}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{91CF1E20-E424-4D3E-8CFC-94115AA2DE71}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$C$1:$E$228</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$G$176</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="391">
   <si>
     <t>Name</t>
   </si>
@@ -167,9 +167,6 @@
     <t>Upload a file to TestProject</t>
   </si>
   <si>
-    <t>Bitrise Snyk scan</t>
-  </si>
-  <si>
     <t>apptest.ai Test</t>
   </si>
   <si>
@@ -554,9 +551,6 @@
     <t>Share Pipeline variables</t>
   </si>
   <si>
-    <t>Test with Snyk</t>
-  </si>
-  <si>
     <t>SonarQube Scanner</t>
   </si>
   <si>
@@ -897,9 +891,6 @@
   </si>
   <si>
     <t>https://bitrise.io/integrations/steps/tslint</t>
-  </si>
-  <si>
-    <t>https://bitrise.io/integrations/steps/unzip</t>
   </si>
   <si>
     <t>https://bitrise.io/integrations/steps/update-jira-issue-field</t>
@@ -966,9 +957,6 @@
     <t xml:space="preserve">Zip a directory and then export the path </t>
   </si>
   <si>
-    <t>See report</t>
-  </si>
-  <si>
     <t>Builds a Pebble project (smartwatch)</t>
   </si>
   <si>
@@ -979,9 +967,6 @@
 https://bitrise.io/integrations/steps/gradle-dependency-checker</t>
   </si>
   <si>
-    <t>Have to be launched after apps-decompiler</t>
-  </si>
-  <si>
     <t>Checks for changing app size</t>
   </si>
   <si>
@@ -993,14 +978,6 @@
 https://bitrise.io/integrations/steps/android-lint</t>
   </si>
   <si>
-    <t>https://snyk.io/
-https://bitrise.io/integrations/steps/bitrise-snyk-scan</t>
-  </si>
-  <si>
-    <t>https://snyk.io/
-https://bitrise.io/integrations/steps/snyk</t>
-  </si>
-  <si>
     <t>https://www.lambdatest.com/
 https://bitrise.io/integrations/steps/lambdatest-upload</t>
   </si>
@@ -1243,11 +1220,6 @@
     <t>Needs local server</t>
   </si>
   <si>
-    <t>See report
-Free trial can't see everything
-9 high and medium vulnerabilities are hidden</t>
-  </si>
-  <si>
     <t>Utility</t>
   </si>
   <si>
@@ -1255,6 +1227,61 @@
   </si>
   <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t>Test with Snyk (Bitrise Snyk scan)</t>
+  </si>
+  <si>
+    <t>https://snyk.io/
+https://bitrise.io/integrations/steps/snyk
+https://bitrise.io/integrations/steps/bitrise-snyk-scan</t>
+  </si>
+  <si>
+    <t>See Report on GitHub</t>
+  </si>
+  <si>
+    <t>Unit tests</t>
+  </si>
+  <si>
+    <t>Code coverage tool</t>
+  </si>
+  <si>
+    <t>Manual testing possible for free, 
+no CI integration</t>
+  </si>
+  <si>
+    <t>Contact developer for pricing, no free version</t>
+  </si>
+  <si>
+    <t>Virtual device testing</t>
+  </si>
+  <si>
+    <t>Contact developer for pricing and free trial</t>
+  </si>
+  <si>
+    <t>No free trial available</t>
+  </si>
+  <si>
+    <t>14 day Free trial 
+UI testing</t>
+  </si>
+  <si>
+    <t>Real/Virtual device testing</t>
+  </si>
+  <si>
+    <t>See Report on GitHub on GitHub</t>
+  </si>
+  <si>
+    <t>Have to be launched after apps-decompiler
+See Report on GitHub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No free version for CI/CD usage
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No free version, request a demo only possibility
+</t>
   </si>
 </sst>
 </file>
@@ -1307,7 +1334,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1326,9 +1353,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1645,11 +1669,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D335C176-F383-4FB8-A686-6624E307DAFB}">
-  <dimension ref="A1:H228"/>
+  <dimension ref="A1:H176"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E171" sqref="E171"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1659,7 +1683,7 @@
     <col min="4" max="4" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="112.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="95" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1667,22 +1691,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="H1" s="4"/>
     </row>
@@ -1691,18 +1715,20 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>378</v>
+      </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1710,22 +1736,22 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>308</v>
+        <v>377</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -1734,22 +1760,22 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>308</v>
+        <v>377</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -1758,16 +1784,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -1776,18 +1802,20 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="G6" s="1"/>
+        <v>313</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>379</v>
+      </c>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1795,18 +1823,20 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="G7" s="1"/>
+        <v>314</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>380</v>
+      </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1814,19 +1844,19 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -1835,18 +1865,20 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1854,18 +1886,20 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1873,19 +1907,19 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -1894,18 +1928,20 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="G12" s="1"/>
+        <v>312</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>382</v>
+      </c>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1913,19 +1949,19 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -1934,18 +1970,20 @@
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="G14" s="1"/>
+        <v>320</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>383</v>
+      </c>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1953,13 +1991,16 @@
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>329</v>
+        <v>322</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>384</v>
       </c>
       <c r="H15" s="1"/>
     </row>
@@ -1968,34 +2009,38 @@
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="G16" s="1"/>
+        <v>321</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>384</v>
+      </c>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>378</v>
+      </c>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2003,38 +2048,40 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="G18" s="1"/>
+        <v>323</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>390</v>
+      </c>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>379</v>
+        <v>324</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>389</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -2043,15 +2090,17 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>55</v>
+        <v>373</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="G20" s="1"/>
+        <v>325</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>384</v>
+      </c>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2059,13 +2108,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H21" s="1"/>
     </row>
@@ -2074,15 +2123,17 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="G22" s="1"/>
+        <v>327</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2090,18 +2141,20 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>335</v>
-      </c>
-      <c r="G23" s="1"/>
+        <v>328</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>379</v>
+      </c>
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2109,15 +2162,17 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="G24" s="1"/>
+        <v>329</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2125,15 +2180,17 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="G25" s="1"/>
+        <v>330</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2141,18 +2198,20 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>338</v>
-      </c>
-      <c r="G26" s="1"/>
+        <v>331</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>377</v>
+      </c>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2160,18 +2219,20 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="G27" s="1"/>
+        <v>332</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2179,18 +2240,17 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="G28" s="1"/>
+        <v>333</v>
+      </c>
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2198,15 +2258,14 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>341</v>
-      </c>
-      <c r="G29" s="1"/>
+        <v>334</v>
+      </c>
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2214,18 +2273,17 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="G30" s="1"/>
+        <v>335</v>
+      </c>
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2233,15 +2291,17 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>343</v>
-      </c>
-      <c r="G31" s="1"/>
+        <v>336</v>
+      </c>
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2249,18 +2309,17 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>344</v>
-      </c>
-      <c r="G32" s="1"/>
+        <v>337</v>
+      </c>
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2268,18 +2327,17 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="G33" s="1"/>
+        <v>338</v>
+      </c>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2287,19 +2345,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H34" s="1"/>
     </row>
@@ -2308,19 +2366,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H35" s="1"/>
     </row>
@@ -2329,18 +2387,17 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>348</v>
-      </c>
-      <c r="G36" s="1"/>
+        <v>341</v>
+      </c>
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2348,19 +2405,19 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H37" s="1"/>
     </row>
@@ -2369,19 +2426,19 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H38" s="1"/>
     </row>
@@ -2390,18 +2447,17 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>351</v>
-      </c>
-      <c r="G39" s="1"/>
+        <v>344</v>
+      </c>
       <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2409,18 +2465,17 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="G40" s="1"/>
+        <v>345</v>
+      </c>
       <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2428,18 +2483,17 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>353</v>
-      </c>
-      <c r="G41" s="1"/>
+        <v>346</v>
+      </c>
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2447,18 +2501,17 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="G42" s="1"/>
+        <v>347</v>
+      </c>
       <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2466,22 +2519,19 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>316</v>
+        <v>348</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>308</v>
+        <v>60</v>
       </c>
       <c r="H43" s="1"/>
     </row>
@@ -2490,19 +2540,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -2511,19 +2561,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>61</v>
+        <v>350</v>
       </c>
       <c r="H45" s="1"/>
     </row>
@@ -2532,91 +2579,86 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="G46" s="1"/>
+        <v>352</v>
+      </c>
       <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>359</v>
-      </c>
-      <c r="G47" s="1"/>
+        <v>351</v>
+      </c>
       <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>358</v>
-      </c>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-    </row>
-    <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>47</v>
-      </c>
       <c r="B49" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>55</v>
+        <v>373</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>360</v>
-      </c>
-      <c r="G49" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G50" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>354</v>
+      </c>
       <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2624,18 +2666,20 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>361</v>
-      </c>
-      <c r="G51" s="1"/>
+        <v>355</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="H51" s="1"/>
     </row>
     <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2643,19 +2687,19 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H52" s="1"/>
     </row>
@@ -2664,19 +2708,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>363</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>61</v>
+        <v>357</v>
       </c>
       <c r="H53" s="1"/>
     </row>
@@ -2685,68 +2723,68 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>364</v>
-      </c>
-      <c r="G54" s="1"/>
+        <v>358</v>
+      </c>
       <c r="H54" s="1"/>
     </row>
     <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>54</v>
+      <c r="A55" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>55</v>
+        <v>372</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
+        <v>359</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -2754,594 +2792,560 @@
         <v>67</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G58" s="1"/>
+        <v>187</v>
+      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G59" s="1"/>
+        <v>188</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G60" s="1"/>
+        <v>189</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G61" s="1"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>368</v>
-      </c>
-      <c r="G63" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G64" s="1"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="G65" s="1"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="G66" s="1"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="G67" s="1"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="G68" s="1"/>
-    </row>
-    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="G69" s="1"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G70" s="1"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G71" s="1"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="G72" s="1"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="G73" s="1"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="G74" s="1"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="G75" s="1"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G76" s="1"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="G77" s="1"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="G78" s="1"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="G79" s="1"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="G80" s="1"/>
-    </row>
-    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F81" s="6" t="s">
-        <v>370</v>
-      </c>
-      <c r="G81" s="1"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G82" s="1"/>
-    </row>
-    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F83" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="G83" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="G84" s="1"/>
+        <v>209</v>
+      </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="G85" s="1"/>
+        <v>210</v>
+      </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="G86" s="1"/>
+        <v>211</v>
+      </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G87" s="1"/>
+        <v>212</v>
+      </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>97</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="G88" s="1"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G89" s="1"/>
-    </row>
-    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>99</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F90" s="6" t="s">
-        <v>372</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>298</v>
+        <v>54</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -3349,55 +3353,53 @@
         <v>100</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="G91" s="1"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="G92" s="1"/>
-    </row>
-    <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>102</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F93" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>299</v>
+        <v>54</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -3405,109 +3407,104 @@
         <v>103</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G94" s="1"/>
+        <v>217</v>
+      </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>104</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="G95" s="1"/>
+        <v>218</v>
+      </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>105</v>
+        <v>183</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="G96" s="1"/>
+        <v>219</v>
+      </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>185</v>
+        <v>105</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="G97" s="1"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="G98" s="1"/>
-    </row>
-    <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="F98" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>107</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F99" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>300</v>
+        <v>54</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3515,129 +3512,127 @@
         <v>108</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="G100" s="1"/>
+        <v>222</v>
+      </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="G101" s="1"/>
+        <v>223</v>
+      </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>110</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="G102" s="1"/>
+        <v>224</v>
+      </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>111</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="G103" s="1"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="G104" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="F104" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="105" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F106" s="6" t="s">
-        <v>376</v>
+        <v>54</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3645,19 +3640,13 @@
         <v>115</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>55</v>
+        <v>372</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="G107" s="1" t="s">
-        <v>302</v>
+        <v>227</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -3665,337 +3654,322 @@
         <v>116</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="G108" s="1"/>
+        <v>228</v>
+      </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>117</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="G109" s="1"/>
+        <v>229</v>
+      </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>118</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="G110" s="1"/>
+        <v>230</v>
+      </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>119</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="G111" s="1"/>
+        <v>231</v>
+      </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>120</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="G112" s="1"/>
+        <v>232</v>
+      </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>121</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="G113" s="1"/>
+        <v>233</v>
+      </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="G114" s="1"/>
+        <v>234</v>
+      </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="G115" s="1"/>
+        <v>235</v>
+      </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="G116" s="1"/>
+        <v>236</v>
+      </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>55</v>
+        <v>372</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="G117" s="1"/>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="G118" s="1"/>
-    </row>
-    <row r="119" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="F118" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>55</v>
+        <v>372</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F119" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="G119" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>128</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G120" s="1"/>
+        <v>239</v>
+      </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>129</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="G121" s="1"/>
+        <v>240</v>
+      </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="G122" s="1"/>
+        <v>241</v>
+      </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>131</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="G123" s="1"/>
+        <v>242</v>
+      </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>132</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="G124" s="1"/>
+        <v>243</v>
+      </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>133</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F125" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="G125" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F126" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="G126" s="1" t="s">
-        <v>303</v>
+        <v>54</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -4003,40 +3977,45 @@
         <v>135</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="G127" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>136</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>312</v>
+        <v>388</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -4044,22 +4023,19 @@
         <v>137</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F129" s="2" t="s">
-        <v>249</v>
+        <v>54</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>248</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -4067,19 +4043,16 @@
         <v>138</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="G130" s="1" t="s">
-        <v>313</v>
+        <v>249</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -4087,55 +4060,56 @@
         <v>139</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="G131" s="1"/>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>140</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="G132" s="1"/>
-    </row>
-    <row r="133" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="F132" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="G132" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>141</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F133" s="5" t="s">
-        <v>304</v>
+        <v>54</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>251</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
@@ -4143,19 +4117,16 @@
         <v>142</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F134" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="G134" s="1" t="s">
-        <v>305</v>
+        <v>54</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -4163,322 +4134,305 @@
         <v>143</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="G135" s="1"/>
+        <v>253</v>
+      </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="G136" s="1"/>
+        <v>254</v>
+      </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="G137" s="1"/>
+        <v>255</v>
+      </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="G138" s="1"/>
+        <v>256</v>
+      </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>147</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="G139" s="1"/>
+        <v>257</v>
+      </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>148</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G140" s="1"/>
+        <v>258</v>
+      </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>149</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="G141" s="1"/>
+        <v>259</v>
+      </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>150</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="G142" s="1"/>
+        <v>260</v>
+      </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>151</v>
+        <v>184</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="G143" s="1"/>
+        <v>261</v>
+      </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="G144" s="1"/>
+        <v>262</v>
+      </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>152</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="G145" s="1"/>
+        <v>263</v>
+      </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>153</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="G146" s="1"/>
+        <v>264</v>
+      </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>154</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>55</v>
+        <v>372</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="G147" s="1"/>
+        <v>265</v>
+      </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>155</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="G148" s="1"/>
+        <v>266</v>
+      </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>156</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="G149" s="1"/>
+        <v>267</v>
+      </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>157</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="G150" s="1"/>
+        <v>268</v>
+      </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>158</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F151" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="G151" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>159</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F152" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="G152" s="1" t="s">
-        <v>306</v>
+        <v>54</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
@@ -4486,637 +4440,446 @@
         <v>160</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="G153" s="1"/>
+        <v>271</v>
+      </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>161</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G154" s="1"/>
+        <v>272</v>
+      </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="G155" s="1"/>
+        <v>273</v>
+      </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>163</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="G156" s="1"/>
+        <v>274</v>
+      </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>164</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="G157" s="1"/>
+        <v>275</v>
+      </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>165</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="G158" s="1"/>
+        <v>276</v>
+      </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>166</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="G159" s="1"/>
+        <v>277</v>
+      </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>167</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="G160" s="1"/>
+        <v>278</v>
+      </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>168</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>55</v>
+        <v>372</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="G161" s="1"/>
+        <v>279</v>
+      </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>169</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="G162" s="1"/>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>170</v>
+        <v>375</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F163" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="G163" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="F163" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G163" s="1" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="164" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F164" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="G164" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B164" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E164" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F164" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="G164" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A165" s="3" t="s">
-        <v>172</v>
-      </c>
       <c r="B165" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F165" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="G165" s="1" t="s">
-        <v>378</v>
+        <v>54</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G166" s="1"/>
+        <v>282</v>
+      </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="G167" s="1"/>
+        <v>283</v>
+      </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>55</v>
+        <v>372</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F168" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="G168" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="F168" s="2" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="G169" s="1"/>
+        <v>284</v>
+      </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="G170" s="1"/>
+        <v>285</v>
+      </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F171" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="G171" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="F171" s="2" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F172" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="G172" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="G173" s="1"/>
+        <v>288</v>
+      </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="G174" s="1"/>
+        <v>289</v>
+      </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="G175" s="1"/>
+        <v>290</v>
+      </c>
+      <c r="G175" s="1" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F176" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="G176" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A177" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E177" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F177" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G178" s="1"/>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G179" s="1"/>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G180" s="1"/>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G181" s="1"/>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G182" s="1"/>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G183" s="1"/>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G184" s="1"/>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G185" s="1"/>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G186" s="1"/>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G187" s="1"/>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G188" s="1"/>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G189" s="1"/>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G190" s="1"/>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G191" s="1"/>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G192" s="1"/>
-    </row>
-    <row r="193" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G193" s="1"/>
-    </row>
-    <row r="194" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G194" s="1"/>
-    </row>
-    <row r="195" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G195" s="1"/>
-    </row>
-    <row r="196" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G196" s="1"/>
-    </row>
-    <row r="197" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G197" s="1"/>
-    </row>
-    <row r="198" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G198" s="1"/>
-    </row>
-    <row r="199" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G199" s="1"/>
-    </row>
-    <row r="200" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G200" s="1"/>
-    </row>
-    <row r="201" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G201" s="1"/>
-    </row>
-    <row r="202" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G202" s="1"/>
-    </row>
-    <row r="203" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G203" s="1"/>
-    </row>
-    <row r="204" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G204" s="1"/>
-    </row>
-    <row r="205" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G205" s="1"/>
-    </row>
-    <row r="206" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G206" s="1"/>
-    </row>
-    <row r="207" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G207" s="1"/>
-    </row>
-    <row r="208" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G208" s="1"/>
-    </row>
-    <row r="209" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G209" s="1"/>
-    </row>
-    <row r="210" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G210" s="1"/>
-    </row>
-    <row r="211" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G211" s="1"/>
-    </row>
-    <row r="212" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G212" s="1"/>
-    </row>
-    <row r="213" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G213" s="1"/>
-    </row>
-    <row r="214" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G214" s="1"/>
-    </row>
-    <row r="215" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G215" s="1"/>
-    </row>
-    <row r="216" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G216" s="1"/>
-    </row>
-    <row r="217" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G217" s="1"/>
-    </row>
-    <row r="218" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G218" s="1"/>
-    </row>
-    <row r="219" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G219" s="1"/>
-    </row>
-    <row r="220" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G220" s="1"/>
-    </row>
-    <row r="221" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G221" s="1"/>
-    </row>
-    <row r="222" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G222" s="1"/>
-    </row>
-    <row r="223" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G223" s="1"/>
-    </row>
-    <row r="224" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G224" s="1"/>
-    </row>
-    <row r="225" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G225" s="1"/>
-    </row>
-    <row r="226" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G226" s="1"/>
-    </row>
-    <row r="227" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G227" s="1"/>
-    </row>
-    <row r="228" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G228" s="1"/>
+        <v>291</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:E228" xr:uid="{D335C176-F383-4FB8-A686-6624E307DAFB}"/>
+  <autoFilter ref="A1:G176" xr:uid="{D335C176-F383-4FB8-A686-6624E307DAFB}"/>
   <hyperlinks>
     <hyperlink ref="F18" r:id="rId1" display="https://www.veracode.com/" xr:uid="{07B2DA99-7D25-4A62-8988-89D2BB25AE31}"/>
     <hyperlink ref="F22" r:id="rId2" display="https://kobiton.com" xr:uid="{917A1FEA-55BE-4CFC-A216-B2E5265E13D1}"/>
     <hyperlink ref="F37" r:id="rId3" display="https://nowsecure.com" xr:uid="{B0E0CCA4-8EF1-45C6-831D-550C786EDEEF}"/>
     <hyperlink ref="F2" r:id="rId4" xr:uid="{EBA8A7AF-7B3D-462D-B050-CF128874B93A}"/>
     <hyperlink ref="F4" r:id="rId5" display="https://developer.android.com/studio/write/lint" xr:uid="{1A9B81CE-11E5-4DB1-919C-A47AC98ADE33}"/>
-    <hyperlink ref="F48" r:id="rId6" display="https://github.com/openstf/devicefarmer" xr:uid="{BB7F3DCB-1C29-4D92-8F93-AB3B8BAA6C38}"/>
-    <hyperlink ref="F46" r:id="rId7" display="https://github.com/openstf/devicefarmer" xr:uid="{50A99DD0-E14D-4304-882B-0EA21D8D4985}"/>
-    <hyperlink ref="F54" r:id="rId8" display="https://qytest.com/" xr:uid="{2839D94F-8CA3-4ACF-AB60-180196E5212E}"/>
-    <hyperlink ref="F51" r:id="rId9" display="https://github.com/detekt/detekt" xr:uid="{D108AFD4-5F70-424E-B26F-F1CED531A7B8}"/>
-    <hyperlink ref="F50" r:id="rId10" xr:uid="{FA8AEB44-F2CC-42BE-A0CB-609314CABD87}"/>
-    <hyperlink ref="F49" r:id="rId11" display="https://docs.aws.amazon.com/devicefarm/latest/developerguide/test-types-android-appium-java-testng.html" xr:uid="{DAD75A31-0FFB-4885-9D35-582B51AAD627}"/>
-    <hyperlink ref="F47" r:id="rId12" display="https://docs.aws.amazon.com/devicefarm/latest/developerguide/test-types-android-appium-java-testng.html" xr:uid="{04649D58-3EEA-4BF1-8637-B9A988ADCA62}"/>
-    <hyperlink ref="F63" r:id="rId13" display="https://aws.amazon.com/secrets-manager/" xr:uid="{619D2BD0-936E-4C27-B89F-A21B74B12E2A}"/>
-    <hyperlink ref="F69" r:id="rId14" display="https://www.browserstack.com/app-automate" xr:uid="{A21543CD-8CBA-477A-8D47-1554345263EB}"/>
-    <hyperlink ref="F57" r:id="rId15" display="https://appium.io/" xr:uid="{881F0B28-6596-40F8-AD7A-9CEDFCC269A2}"/>
-    <hyperlink ref="F93" r:id="rId16" display="https://fastlane.tools/" xr:uid="{77E14259-AD65-4878-B97C-E72BC6CD142D}"/>
+    <hyperlink ref="F47" r:id="rId6" display="https://github.com/openstf/devicefarmer" xr:uid="{BB7F3DCB-1C29-4D92-8F93-AB3B8BAA6C38}"/>
+    <hyperlink ref="F45" r:id="rId7" display="https://github.com/openstf/devicefarmer" xr:uid="{50A99DD0-E14D-4304-882B-0EA21D8D4985}"/>
+    <hyperlink ref="F53" r:id="rId8" display="https://qytest.com/" xr:uid="{2839D94F-8CA3-4ACF-AB60-180196E5212E}"/>
+    <hyperlink ref="F50" r:id="rId9" display="https://github.com/detekt/detekt" xr:uid="{D108AFD4-5F70-424E-B26F-F1CED531A7B8}"/>
+    <hyperlink ref="F49" r:id="rId10" xr:uid="{FA8AEB44-F2CC-42BE-A0CB-609314CABD87}"/>
+    <hyperlink ref="F48" r:id="rId11" display="https://docs.aws.amazon.com/devicefarm/latest/developerguide/test-types-android-appium-java-testng.html" xr:uid="{DAD75A31-0FFB-4885-9D35-582B51AAD627}"/>
+    <hyperlink ref="F46" r:id="rId12" display="https://docs.aws.amazon.com/devicefarm/latest/developerguide/test-types-android-appium-java-testng.html" xr:uid="{04649D58-3EEA-4BF1-8637-B9A988ADCA62}"/>
+    <hyperlink ref="F62" r:id="rId13" display="https://aws.amazon.com/secrets-manager/" xr:uid="{619D2BD0-936E-4C27-B89F-A21B74B12E2A}"/>
+    <hyperlink ref="F68" r:id="rId14" display="https://www.browserstack.com/app-automate" xr:uid="{A21543CD-8CBA-477A-8D47-1554345263EB}"/>
+    <hyperlink ref="F56" r:id="rId15" display="https://appium.io/" xr:uid="{881F0B28-6596-40F8-AD7A-9CEDFCC269A2}"/>
+    <hyperlink ref="F92" r:id="rId16" display="https://fastlane.tools/" xr:uid="{77E14259-AD65-4878-B97C-E72BC6CD142D}"/>
     <hyperlink ref="F8" r:id="rId17" display="https://danger.systems/kotlin/" xr:uid="{33A0E697-97DE-412B-9239-FF934228CA03}"/>
     <hyperlink ref="F13" r:id="rId18" display="https://maestro.mobile.dev/" xr:uid="{E6CC59B1-8419-44E7-A9E9-C6C03B81A1E2}"/>
-    <hyperlink ref="F126" r:id="rId19" xr:uid="{7AC0C2FD-8A08-4579-ADF5-49092E58EC89}"/>
-    <hyperlink ref="F133" r:id="rId20" display="https://bitrise.io/integrations/steps/pebble-build" xr:uid="{F09A1D25-E423-4B74-B15A-C628E20A23EB}"/>
-    <hyperlink ref="F134" r:id="rId21" xr:uid="{3C6E9DC9-54A8-49F3-872D-E17FCED6192F}"/>
-    <hyperlink ref="F152" r:id="rId22" xr:uid="{D7332159-6534-4853-BFCE-DF7B15E6A093}"/>
-    <hyperlink ref="F172" r:id="rId23" xr:uid="{B6B23C0B-7E5C-4920-8BB7-3EF19560DFB8}"/>
-    <hyperlink ref="F128" r:id="rId24" xr:uid="{6E503C62-C67B-4667-A56F-044246E167AE}"/>
-    <hyperlink ref="F129" r:id="rId25" xr:uid="{ABA37ABD-9E8D-4522-A523-44FE6995A0AD}"/>
+    <hyperlink ref="F125" r:id="rId19" xr:uid="{7AC0C2FD-8A08-4579-ADF5-49092E58EC89}"/>
+    <hyperlink ref="F132" r:id="rId20" display="https://bitrise.io/integrations/steps/pebble-build" xr:uid="{F09A1D25-E423-4B74-B15A-C628E20A23EB}"/>
+    <hyperlink ref="F133" r:id="rId21" xr:uid="{3C6E9DC9-54A8-49F3-872D-E17FCED6192F}"/>
+    <hyperlink ref="F151" r:id="rId22" xr:uid="{D7332159-6534-4853-BFCE-DF7B15E6A093}"/>
+    <hyperlink ref="F171" r:id="rId23" xr:uid="{B6B23C0B-7E5C-4920-8BB7-3EF19560DFB8}"/>
+    <hyperlink ref="F127" r:id="rId24" xr:uid="{6E503C62-C67B-4667-A56F-044246E167AE}"/>
+    <hyperlink ref="F128" r:id="rId25" xr:uid="{ABA37ABD-9E8D-4522-A523-44FE6995A0AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>

</xml_diff>